<commit_message>
mitsubishi and tamagawa encoders improvements
</commit_message>
<xml_diff>
--- a/servo401/parameter_set.xlsx
+++ b/servo401/parameter_set.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="102">
   <si>
     <t>Error register</t>
   </si>
@@ -326,17 +326,6 @@
 1st order filter (40057)</t>
   </si>
   <si>
-    <t>Actual error, write 0 to acknowledge
-1-Undervolatage
-2-Overvoltage
-3-Output shortcircuit/current transducer error
-4- Inverter Overcurrent
-5- Motor Overcurrent
-6- encoder error
-7- Internal error
-8-external trip by user</t>
-  </si>
-  <si>
     <t>Control/status register</t>
   </si>
   <si>
@@ -358,6 +347,21 @@
   </si>
   <si>
     <t>Field setpoint*10</t>
+  </si>
+  <si>
+    <t>Actual motor voltage*10</t>
+  </si>
+  <si>
+    <t>Actual motor voltage vector length</t>
+  </si>
+  <si>
+    <t>Actual error, write 0 to acknowledge</t>
+  </si>
+  <si>
+    <t>Encoder acceleration error</t>
+  </si>
+  <si>
+    <t>Number of encoder position errors detected</t>
   </si>
 </sst>
 </file>
@@ -805,10 +809,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -862,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -870,7 +874,7 @@
         <v>40003</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -921,10 +925,10 @@
         <v>40007</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>93</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>4</v>
@@ -938,10 +942,10 @@
         <v>40008</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1083,7 +1087,7 @@
         <v>40017</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>17</v>
@@ -1092,177 +1096,177 @@
         <v>18</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>40018</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="12"/>
-    </row>
-    <row r="19" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>40020</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="4" t="s">
+      <c r="D20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>40021</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
+        <v>40021</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>40022</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E21" s="4" t="s">
+      <c r="D22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>40031</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>40032</v>
+        <v>40023</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>31</v>
+        <v>100</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>40033</v>
+        <v>40031</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>37</v>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>40034</v>
+        <v>40032</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>40035</v>
+        <v>40033</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>70</v>
+      <c r="E26" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>40036</v>
+        <v>40034</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>40037</v>
+        <v>40035</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
@@ -1271,125 +1275,125 @@
         <v>4</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
+        <v>40036</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>40037</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>40038</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="2" t="s">
+      <c r="C31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>40039</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>40040</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
+        <v>40039</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>40040</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>40041</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B34" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="4" t="s">
+      <c r="C34" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="8" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
-        <v>40050</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
-        <v>40051</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>40052</v>
+        <v>40050</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>17</v>
@@ -1398,32 +1402,32 @@
         <v>4</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>40053</v>
+        <v>40051</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>40054</v>
+        <v>40052</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>17</v>
@@ -1432,32 +1436,32 @@
         <v>4</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>40055</v>
+        <v>40053</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>66</v>
+        <v>17</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>4</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>40056</v>
+        <v>40054</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>17</v>
@@ -1466,30 +1470,64 @@
         <v>4</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
+        <v>40055</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40056</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
         <v>40057</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B43" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E41" s="4" t="s">
+      <c r="C43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="A2:E2"/>
   </mergeCells>
   <pageMargins left="0.43307086614173229" right="0.43307086614173229" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>

</xml_diff>